<commit_message>
Trocado qual a tela que executa primeiro. Ajustado tela de login Ajustado tela de cadastro Ajustado menu. Criado classe de sessão. Atualizado planilha de tarefas pendentes.
</commit_message>
<xml_diff>
--- a/Cronograma Atual.xlsx
+++ b/Cronograma Atual.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel Wolf\Documents\sistemadecontroledecarros\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9795"/>
   </bookViews>
@@ -12,6 +17,7 @@
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
@@ -123,8 +129,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,13 +145,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -244,7 +262,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -253,10 +271,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -265,20 +280,41 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -316,9 +352,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,9 +386,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -384,9 +438,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -559,14 +631,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
@@ -575,7 +647,7 @@
     <col min="6" max="6" width="56.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,17 +667,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="13">
         <v>43000</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="13">
         <v>43028</v>
       </c>
       <c r="E2" s="5"/>
@@ -613,71 +685,71 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="19">
         <v>43002</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="19">
         <v>43007</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="18"/>
+      <c r="F3" s="20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="23">
         <v>43000</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="23">
         <v>43001</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="22"/>
+      <c r="F4" s="24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="23">
         <v>43007</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="23">
         <v>43013</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="14">
         <v>43007</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="13">
         <v>42983</v>
       </c>
       <c r="E6" s="5"/>
@@ -685,17 +757,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="13">
         <v>43000</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="13">
         <v>43007</v>
       </c>
       <c r="E7" s="5"/>
@@ -703,7 +775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -715,7 +787,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -727,56 +799,56 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="27">
         <v>43001</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="27">
         <v>43007</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11" t="s">
+      <c r="E10" s="28"/>
+      <c r="F10" s="29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="16">
         <v>43002</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="16">
         <v>43002</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="14" t="s">
+      <c r="E11" s="8"/>
+      <c r="F11" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="15">
         <v>43000</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="15">
         <v>43013</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -787,24 +859,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>